<commit_message>
Add seb and seh to decoder.v and decode-table.Change the suc and fail in test/src/trap.h. --dhr
</commit_message>
<xml_diff>
--- a/doc/decoder/流水线CPU译码器信号表-1月7日更新.xlsx
+++ b/doc/decoder/流水线CPU译码器信号表-1月7日更新.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Course\ComputerArctecture\实验\流水线CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bingo\Documents\Tencent Files\1612723830\FileRecv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="198">
   <si>
     <t>指令类型</t>
   </si>
@@ -856,6 +856,38 @@
   </si>
   <si>
     <t>2017/1/7更新</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEB</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1010</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1011</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEH</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1039,7 +1071,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1274,6 +1306,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1297,7 +1338,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1452,6 +1493,10 @@
     <xf numFmtId="49" fontId="9" fillId="10" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1467,8 +1512,6 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="19" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="TableStyleLight1" xfId="2"/>
@@ -1824,12 +1867,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG80"/>
+  <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A82" sqref="A82"/>
-      <selection pane="topRight" activeCell="AB80" sqref="AB80"/>
+      <selection pane="topRight" activeCell="B39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1959,7 +2002,7 @@
       </c>
     </row>
     <row r="2" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="74" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="18" t="s">
@@ -2040,7 +2083,7 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="25" t="s">
         <v>30</v>
       </c>
@@ -2119,7 +2162,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="25" t="s">
         <v>32</v>
       </c>
@@ -2200,7 +2243,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="25" t="s">
         <v>35</v>
       </c>
@@ -2281,7 +2324,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A6" s="70"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="25" t="s">
         <v>36</v>
       </c>
@@ -2360,7 +2403,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="25" t="s">
         <v>38</v>
       </c>
@@ -2439,7 +2482,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="25" t="s">
         <v>40</v>
       </c>
@@ -2518,7 +2561,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A9" s="70"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="25" t="s">
         <v>42</v>
       </c>
@@ -2599,7 +2642,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A10" s="70"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="25" t="s">
         <v>43</v>
       </c>
@@ -2678,7 +2721,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A11" s="70"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="25" t="s">
         <v>45</v>
       </c>
@@ -2759,7 +2802,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A12" s="70"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="25" t="s">
         <v>46</v>
       </c>
@@ -2838,7 +2881,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A13" s="70"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="25" t="s">
         <v>48</v>
       </c>
@@ -2919,7 +2962,7 @@
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A14" s="70"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="25" t="s">
         <v>49</v>
       </c>
@@ -2998,7 +3041,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="70"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="25" t="s">
         <v>51</v>
       </c>
@@ -3077,7 +3120,7 @@
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="25" t="s">
         <v>53</v>
       </c>
@@ -3156,7 +3199,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A17" s="70"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="25" t="s">
         <v>55</v>
       </c>
@@ -3237,7 +3280,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A18" s="70"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="28" t="s">
         <v>56</v>
       </c>
@@ -3318,7 +3361,7 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="76" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -3403,7 +3446,7 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A20" s="72"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="25" t="s">
         <v>61</v>
       </c>
@@ -3484,7 +3527,7 @@
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A21" s="72"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="25" t="s">
         <v>62</v>
       </c>
@@ -3567,7 +3610,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A22" s="72"/>
+      <c r="A22" s="76"/>
       <c r="B22" s="25" t="s">
         <v>63</v>
       </c>
@@ -3648,7 +3691,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A23" s="72"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="25" t="s">
         <v>64</v>
       </c>
@@ -3731,7 +3774,7 @@
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A24" s="72"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="25" t="s">
         <v>66</v>
       </c>
@@ -3812,7 +3855,7 @@
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="74" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -3893,74 +3936,74 @@
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A26" s="70"/>
-      <c r="B26" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="30">
-        <v>0</v>
-      </c>
-      <c r="E26" s="30">
-        <v>0</v>
-      </c>
-      <c r="F26" s="30">
-        <v>0</v>
-      </c>
-      <c r="G26" s="33">
-        <v>1</v>
-      </c>
-      <c r="H26" s="30">
-        <v>0</v>
-      </c>
-      <c r="I26" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="J26" s="30">
-        <v>0</v>
-      </c>
-      <c r="K26" s="31" t="s">
-        <v>71</v>
+      <c r="A26" s="74"/>
+      <c r="B26" s="73" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="38">
+        <v>0</v>
+      </c>
+      <c r="E26" s="38">
+        <v>0</v>
+      </c>
+      <c r="F26" s="38">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="38">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" s="38">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="L26" s="23"/>
       <c r="M26" s="24"/>
       <c r="N26" s="23"/>
       <c r="O26" s="23"/>
       <c r="P26" s="23"/>
-      <c r="Q26" s="30">
+      <c r="Q26" s="38">
         <v>0</v>
       </c>
       <c r="R26" s="24"/>
-      <c r="S26" s="30">
-        <v>0</v>
-      </c>
-      <c r="T26" s="30">
-        <v>0</v>
-      </c>
-      <c r="U26" s="30">
-        <v>0</v>
-      </c>
-      <c r="V26" s="30">
-        <v>0</v>
-      </c>
-      <c r="W26" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="X26" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="30">
+      <c r="S26" s="38">
+        <v>0</v>
+      </c>
+      <c r="T26" s="38">
+        <v>0</v>
+      </c>
+      <c r="U26" s="38">
+        <v>0</v>
+      </c>
+      <c r="V26" s="38">
+        <v>0</v>
+      </c>
+      <c r="W26" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="X26" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="38">
         <v>1</v>
       </c>
       <c r="AA26" s="23"/>
-      <c r="AB26" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC26" s="61" t="s">
-        <v>162</v>
+      <c r="AB26" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
       </c>
       <c r="AD26" s="42"/>
       <c r="AE26" s="38">
@@ -3972,73 +4015,73 @@
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A27" s="72" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20">
-        <v>0</v>
-      </c>
-      <c r="E27" s="20">
-        <v>0</v>
-      </c>
-      <c r="F27" s="20">
-        <v>0</v>
-      </c>
-      <c r="G27" s="21">
-        <v>0</v>
-      </c>
-      <c r="H27" s="20">
-        <v>1</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27" s="20">
-        <v>0</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>39</v>
+      <c r="A27" s="74"/>
+      <c r="B27" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="72"/>
+      <c r="D27" s="38">
+        <v>0</v>
+      </c>
+      <c r="E27" s="38">
+        <v>0</v>
+      </c>
+      <c r="F27" s="38">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="38">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J27" s="38">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="L27" s="23"/>
       <c r="M27" s="24"/>
       <c r="N27" s="23"/>
       <c r="O27" s="23"/>
       <c r="P27" s="23"/>
-      <c r="Q27" s="20">
+      <c r="Q27" s="38">
         <v>0</v>
       </c>
       <c r="R27" s="24"/>
-      <c r="S27" s="20">
-        <v>0</v>
-      </c>
-      <c r="T27" s="20">
-        <v>0</v>
-      </c>
-      <c r="U27" s="20">
-        <v>0</v>
-      </c>
-      <c r="V27" s="20">
-        <v>0</v>
-      </c>
-      <c r="W27" s="57"/>
-      <c r="X27" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB27" s="43"/>
-      <c r="AC27" s="18">
+      <c r="S27" s="38">
+        <v>0</v>
+      </c>
+      <c r="T27" s="38">
+        <v>0</v>
+      </c>
+      <c r="U27" s="38">
+        <v>0</v>
+      </c>
+      <c r="V27" s="38">
+        <v>0</v>
+      </c>
+      <c r="W27" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="X27" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="23"/>
+      <c r="AB27" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC27">
         <v>0</v>
       </c>
       <c r="AD27" s="42"/>
@@ -4051,72 +4094,74 @@
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A28" s="72"/>
-      <c r="B28" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>39</v>
+      <c r="A28" s="74"/>
+      <c r="B28" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30">
+        <v>0</v>
+      </c>
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="G28" s="33">
+        <v>1</v>
+      </c>
+      <c r="H28" s="30">
+        <v>0</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="30">
+        <v>0</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>71</v>
       </c>
       <c r="L28" s="23"/>
       <c r="M28" s="24"/>
       <c r="N28" s="23"/>
       <c r="O28" s="23"/>
       <c r="P28" s="23"/>
-      <c r="Q28" s="2">
+      <c r="Q28" s="30">
         <v>0</v>
       </c>
       <c r="R28" s="24"/>
-      <c r="S28" s="2">
-        <v>0</v>
-      </c>
-      <c r="T28" s="2">
-        <v>0</v>
-      </c>
-      <c r="U28" s="2">
-        <v>0</v>
-      </c>
-      <c r="V28" s="2">
-        <v>0</v>
-      </c>
-      <c r="W28" s="57"/>
-      <c r="X28" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA28" s="4" t="s">
+      <c r="S28" s="30">
+        <v>0</v>
+      </c>
+      <c r="T28" s="30">
+        <v>0</v>
+      </c>
+      <c r="U28" s="30">
+        <v>0</v>
+      </c>
+      <c r="V28" s="30">
+        <v>0</v>
+      </c>
+      <c r="W28" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="X28" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AB28" s="43"/>
-      <c r="AC28" s="25">
-        <v>0</v>
+      <c r="AC28" s="61" t="s">
+        <v>162</v>
       </c>
       <c r="AD28" s="42"/>
       <c r="AE28" s="38">
@@ -4128,33 +4173,35 @@
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A29" s="72"/>
-      <c r="B29" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J29" s="2">
-        <v>0</v>
-      </c>
-      <c r="K29" s="4" t="s">
+      <c r="A29" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20">
+        <v>0</v>
+      </c>
+      <c r="E29" s="20">
+        <v>0</v>
+      </c>
+      <c r="F29" s="20">
+        <v>0</v>
+      </c>
+      <c r="G29" s="21">
+        <v>0</v>
+      </c>
+      <c r="H29" s="20">
+        <v>1</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="J29" s="20">
+        <v>0</v>
+      </c>
+      <c r="K29" s="22" t="s">
         <v>39</v>
       </c>
       <c r="L29" s="23"/>
@@ -4162,38 +4209,38 @@
       <c r="N29" s="23"/>
       <c r="O29" s="23"/>
       <c r="P29" s="23"/>
-      <c r="Q29" s="2">
+      <c r="Q29" s="20">
         <v>0</v>
       </c>
       <c r="R29" s="24"/>
-      <c r="S29" s="2">
-        <v>0</v>
-      </c>
-      <c r="T29" s="2">
-        <v>0</v>
-      </c>
-      <c r="U29" s="2">
-        <v>0</v>
-      </c>
-      <c r="V29" s="2">
+      <c r="S29" s="20">
+        <v>0</v>
+      </c>
+      <c r="T29" s="20">
+        <v>0</v>
+      </c>
+      <c r="U29" s="20">
+        <v>0</v>
+      </c>
+      <c r="V29" s="20">
         <v>0</v>
       </c>
       <c r="W29" s="57"/>
-      <c r="X29" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="4" t="s">
-        <v>29</v>
+      <c r="X29" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="20">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="22" t="s">
+        <v>160</v>
       </c>
       <c r="AB29" s="43"/>
-      <c r="AC29" s="25">
-        <v>1</v>
+      <c r="AC29" s="18">
+        <v>0</v>
       </c>
       <c r="AD29" s="42"/>
       <c r="AE29" s="38">
@@ -4205,9 +4252,9 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A30" s="72"/>
-      <c r="B30" s="25" t="s">
-        <v>76</v>
+      <c r="A30" s="76"/>
+      <c r="B30" s="63" t="s">
+        <v>73</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" s="2">
@@ -4226,7 +4273,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="J30" s="2">
         <v>0</v>
@@ -4270,7 +4317,7 @@
       </c>
       <c r="AB30" s="43"/>
       <c r="AC30" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD30" s="42"/>
       <c r="AE30" s="38">
@@ -4282,9 +4329,9 @@
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A31" s="72"/>
+      <c r="A31" s="76"/>
       <c r="B31" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C31" s="27"/>
       <c r="D31" s="2">
@@ -4303,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J31" s="2">
         <v>0</v>
@@ -4359,9 +4406,9 @@
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A32" s="72"/>
+      <c r="A32" s="76"/>
       <c r="B32" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="2">
@@ -4380,7 +4427,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J32" s="2">
         <v>0</v>
@@ -4436,11 +4483,11 @@
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A33" s="72"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="32"/>
+        <v>78</v>
+      </c>
+      <c r="C33" s="27"/>
       <c r="D33" s="2">
         <v>0</v>
       </c>
@@ -4457,7 +4504,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J33" s="2">
         <v>0</v>
@@ -4501,7 +4548,7 @@
       </c>
       <c r="AB33" s="43"/>
       <c r="AC33" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33" s="42"/>
       <c r="AE33" s="38">
@@ -4513,76 +4560,76 @@
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A34" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="38">
-        <v>0</v>
-      </c>
-      <c r="E34" s="38">
-        <v>0</v>
-      </c>
-      <c r="F34" s="38">
+      <c r="A34" s="76"/>
+      <c r="B34" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
         <v>0</v>
       </c>
       <c r="G34" s="3">
         <v>0</v>
       </c>
-      <c r="H34" s="38">
-        <v>0</v>
-      </c>
-      <c r="I34" s="67" t="s">
-        <v>174</v>
-      </c>
-      <c r="J34" s="38">
+      <c r="H34" s="2">
+        <v>1</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J34" s="2">
         <v>0</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="L34" s="23"/>
       <c r="M34" s="24"/>
       <c r="N34" s="23"/>
       <c r="O34" s="23"/>
       <c r="P34" s="23"/>
-      <c r="Q34" s="38">
+      <c r="Q34" s="2">
         <v>0</v>
       </c>
       <c r="R34" s="24"/>
-      <c r="S34" s="38">
-        <v>0</v>
-      </c>
-      <c r="T34" s="38">
-        <v>0</v>
-      </c>
-      <c r="U34" s="38">
-        <v>0</v>
-      </c>
-      <c r="V34" s="38">
-        <v>0</v>
-      </c>
-      <c r="W34" s="47"/>
-      <c r="X34" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="45"/>
+      <c r="S34" s="2">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>0</v>
+      </c>
+      <c r="U34" s="2">
+        <v>0</v>
+      </c>
+      <c r="V34" s="2">
+        <v>0</v>
+      </c>
+      <c r="W34" s="57"/>
+      <c r="X34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AB34" s="43"/>
-      <c r="AC34" s="38">
-        <v>0</v>
+      <c r="AC34" s="25">
+        <v>1</v>
       </c>
       <c r="AD34" s="42"/>
       <c r="AE34" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF34" s="45"/>
       <c r="AG34" s="38">
@@ -4590,74 +4637,76 @@
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A35" s="73"/>
-      <c r="B35" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="38">
-        <v>0</v>
-      </c>
-      <c r="E35" s="38">
-        <v>0</v>
-      </c>
-      <c r="F35" s="38">
+      <c r="A35" s="76"/>
+      <c r="B35" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="32"/>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
         <v>0</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
       </c>
-      <c r="H35" s="38">
-        <v>0</v>
-      </c>
-      <c r="I35" s="67" t="s">
-        <v>175</v>
-      </c>
-      <c r="J35" s="38">
-        <v>1</v>
+      <c r="H35" s="2">
+        <v>1</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="L35" s="23"/>
       <c r="M35" s="24"/>
       <c r="N35" s="23"/>
       <c r="O35" s="23"/>
       <c r="P35" s="23"/>
-      <c r="Q35" s="38">
+      <c r="Q35" s="2">
         <v>0</v>
       </c>
       <c r="R35" s="24"/>
-      <c r="S35" s="38">
-        <v>0</v>
-      </c>
-      <c r="T35" s="38">
-        <v>0</v>
-      </c>
-      <c r="U35" s="38">
-        <v>0</v>
-      </c>
-      <c r="V35" s="38">
-        <v>0</v>
-      </c>
-      <c r="W35" s="47"/>
-      <c r="X35" s="38">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="38">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="38">
+      <c r="S35" s="2">
+        <v>0</v>
+      </c>
+      <c r="T35" s="2">
+        <v>0</v>
+      </c>
+      <c r="U35" s="2">
+        <v>0</v>
+      </c>
+      <c r="V35" s="2">
+        <v>0</v>
+      </c>
+      <c r="W35" s="57"/>
+      <c r="X35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="2">
         <v>1</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>146</v>
+        <v>29</v>
       </c>
       <c r="AB35" s="43"/>
-      <c r="AC35" s="45"/>
+      <c r="AC35" s="25">
+        <v>0</v>
+      </c>
       <c r="AD35" s="42"/>
       <c r="AE35" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF35" s="45"/>
       <c r="AG35" s="38">
@@ -4665,9 +4714,11 @@
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A36" s="73"/>
+      <c r="A36" s="76" t="s">
+        <v>129</v>
+      </c>
       <c r="B36" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C36" s="44"/>
       <c r="D36" s="38">
@@ -4686,13 +4737,13 @@
         <v>0</v>
       </c>
       <c r="I36" s="67" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J36" s="38">
         <v>0</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="L36" s="23"/>
       <c r="M36" s="24"/>
@@ -4740,9 +4791,9 @@
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A37" s="73"/>
+      <c r="A37" s="77"/>
       <c r="B37" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C37" s="44"/>
       <c r="D37" s="38">
@@ -4761,13 +4812,13 @@
         <v>0</v>
       </c>
       <c r="I37" s="67" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J37" s="38">
         <v>1</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>39</v>
+        <v>142</v>
       </c>
       <c r="L37" s="23"/>
       <c r="M37" s="24"/>
@@ -4801,7 +4852,7 @@
         <v>1</v>
       </c>
       <c r="AA37" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AB37" s="43"/>
       <c r="AC37" s="45"/>
@@ -4815,9 +4866,9 @@
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A38" s="73"/>
+      <c r="A38" s="77"/>
       <c r="B38" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C38" s="44"/>
       <c r="D38" s="38">
@@ -4836,13 +4887,13 @@
         <v>0</v>
       </c>
       <c r="I38" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J38" s="38">
         <v>0</v>
       </c>
-      <c r="K38" s="57" t="s">
-        <v>182</v>
+      <c r="K38" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="L38" s="23"/>
       <c r="M38" s="24"/>
@@ -4890,9 +4941,9 @@
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A39" s="73"/>
+      <c r="A39" s="77"/>
       <c r="B39" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="38">
@@ -4911,13 +4962,13 @@
         <v>0</v>
       </c>
       <c r="I39" s="67" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J39" s="38">
         <v>1</v>
       </c>
-      <c r="K39" s="57" t="s">
-        <v>183</v>
+      <c r="K39" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="L39" s="23"/>
       <c r="M39" s="24"/>
@@ -4951,7 +5002,7 @@
         <v>1</v>
       </c>
       <c r="AA39" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AB39" s="43"/>
       <c r="AC39" s="45"/>
@@ -4965,9 +5016,9 @@
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A40" s="73"/>
+      <c r="A40" s="77"/>
       <c r="B40" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C40" s="44"/>
       <c r="D40" s="38">
@@ -4986,13 +5037,13 @@
         <v>0</v>
       </c>
       <c r="I40" s="67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J40" s="38">
         <v>0</v>
       </c>
-      <c r="K40" s="4" t="s">
-        <v>39</v>
+      <c r="K40" s="57" t="s">
+        <v>182</v>
       </c>
       <c r="L40" s="23"/>
       <c r="M40" s="24"/>
@@ -5040,9 +5091,9 @@
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A41" s="73"/>
+      <c r="A41" s="77"/>
       <c r="B41" s="38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C41" s="44"/>
       <c r="D41" s="38">
@@ -5061,13 +5112,13 @@
         <v>0</v>
       </c>
       <c r="I41" s="67" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J41" s="38">
         <v>1</v>
       </c>
-      <c r="K41" s="4" t="s">
-        <v>39</v>
+      <c r="K41" s="57" t="s">
+        <v>183</v>
       </c>
       <c r="L41" s="23"/>
       <c r="M41" s="24"/>
@@ -5101,7 +5152,7 @@
         <v>1</v>
       </c>
       <c r="AA41" s="4" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AB41" s="43"/>
       <c r="AC41" s="45"/>
@@ -5115,9 +5166,9 @@
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A42" s="73"/>
+      <c r="A42" s="77"/>
       <c r="B42" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C42" s="44"/>
       <c r="D42" s="38">
@@ -5141,8 +5192,8 @@
       <c r="J42" s="38">
         <v>0</v>
       </c>
-      <c r="K42" s="57" t="s">
-        <v>182</v>
+      <c r="K42" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="L42" s="23"/>
       <c r="M42" s="24"/>
@@ -5190,9 +5241,9 @@
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A43" s="73"/>
+      <c r="A43" s="77"/>
       <c r="B43" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="38">
@@ -5216,8 +5267,8 @@
       <c r="J43" s="38">
         <v>1</v>
       </c>
-      <c r="K43" s="57" t="s">
-        <v>184</v>
+      <c r="K43" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="L43" s="23"/>
       <c r="M43" s="24"/>
@@ -5265,9 +5316,9 @@
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A44" s="73"/>
+      <c r="A44" s="77"/>
       <c r="B44" s="38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C44" s="44"/>
       <c r="D44" s="38">
@@ -5286,13 +5337,13 @@
         <v>0</v>
       </c>
       <c r="I44" s="67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J44" s="38">
         <v>0</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>39</v>
+      <c r="K44" s="57" t="s">
+        <v>182</v>
       </c>
       <c r="L44" s="23"/>
       <c r="M44" s="24"/>
@@ -5340,9 +5391,9 @@
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A45" s="74"/>
+      <c r="A45" s="77"/>
       <c r="B45" s="38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="38">
@@ -5361,13 +5412,13 @@
         <v>0</v>
       </c>
       <c r="I45" s="67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J45" s="38">
         <v>1</v>
       </c>
-      <c r="K45" s="4" t="s">
-        <v>39</v>
+      <c r="K45" s="57" t="s">
+        <v>184</v>
       </c>
       <c r="L45" s="23"/>
       <c r="M45" s="24"/>
@@ -5401,7 +5452,7 @@
         <v>1</v>
       </c>
       <c r="AA45" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AB45" s="43"/>
       <c r="AC45" s="45"/>
@@ -5415,72 +5466,74 @@
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A46" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="34">
-        <v>1</v>
-      </c>
-      <c r="E46" s="34">
-        <v>0</v>
-      </c>
-      <c r="F46" s="34">
-        <v>0</v>
-      </c>
-      <c r="G46" s="36">
-        <v>0</v>
-      </c>
-      <c r="H46" s="34">
-        <v>0</v>
-      </c>
-      <c r="I46" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="J46" s="34">
-        <v>0</v>
-      </c>
-      <c r="K46" s="23"/>
+      <c r="A46" s="77"/>
+      <c r="B46" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="44"/>
+      <c r="D46" s="38">
+        <v>0</v>
+      </c>
+      <c r="E46" s="38">
+        <v>0</v>
+      </c>
+      <c r="F46" s="38">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="38">
+        <v>0</v>
+      </c>
+      <c r="I46" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="J46" s="38">
+        <v>0</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="L46" s="23"/>
       <c r="M46" s="24"/>
       <c r="N46" s="23"/>
       <c r="O46" s="23"/>
       <c r="P46" s="23"/>
-      <c r="Q46" s="34">
+      <c r="Q46" s="38">
         <v>0</v>
       </c>
       <c r="R46" s="24"/>
-      <c r="S46" s="34">
-        <v>0</v>
-      </c>
-      <c r="T46" s="34">
-        <v>0</v>
-      </c>
-      <c r="U46" s="34">
-        <v>0</v>
-      </c>
-      <c r="V46" s="34">
+      <c r="S46" s="38">
+        <v>0</v>
+      </c>
+      <c r="T46" s="38">
+        <v>0</v>
+      </c>
+      <c r="U46" s="38">
+        <v>0</v>
+      </c>
+      <c r="V46" s="38">
         <v>0</v>
       </c>
       <c r="W46" s="47"/>
-      <c r="X46" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="62">
-        <v>1</v>
-      </c>
-      <c r="AA46" s="23"/>
-      <c r="AB46" s="23"/>
-      <c r="AC46" s="24"/>
+      <c r="X46" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="45"/>
+      <c r="AB46" s="43"/>
+      <c r="AC46" s="38">
+        <v>0</v>
+      </c>
       <c r="AD46" s="42"/>
-      <c r="AE46" s="2">
-        <v>0</v>
+      <c r="AE46" s="38">
+        <v>1</v>
       </c>
       <c r="AF46" s="45"/>
       <c r="AG46" s="38">
@@ -5488,78 +5541,74 @@
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A47" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="20">
-        <v>1</v>
-      </c>
-      <c r="E47" s="20">
-        <v>0</v>
-      </c>
-      <c r="F47" s="20">
-        <v>0</v>
-      </c>
-      <c r="G47" s="50">
-        <v>1</v>
-      </c>
-      <c r="H47" s="20">
-        <v>0</v>
-      </c>
-      <c r="I47" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J47" s="20">
-        <v>0</v>
-      </c>
-      <c r="K47" s="23"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="44"/>
+      <c r="D47" s="38">
+        <v>0</v>
+      </c>
+      <c r="E47" s="38">
+        <v>0</v>
+      </c>
+      <c r="F47" s="38">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="38">
+        <v>0</v>
+      </c>
+      <c r="I47" s="67" t="s">
+        <v>180</v>
+      </c>
+      <c r="J47" s="38">
+        <v>1</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="L47" s="23"/>
       <c r="M47" s="24"/>
       <c r="N47" s="23"/>
       <c r="O47" s="23"/>
       <c r="P47" s="23"/>
-      <c r="Q47" s="20">
+      <c r="Q47" s="38">
         <v>0</v>
       </c>
       <c r="R47" s="24"/>
-      <c r="S47" s="20">
-        <v>0</v>
-      </c>
-      <c r="T47" s="20">
-        <v>0</v>
-      </c>
-      <c r="U47" s="20">
-        <v>0</v>
-      </c>
-      <c r="V47" s="20">
-        <v>0</v>
-      </c>
-      <c r="W47" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="X47" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="62">
-        <v>1</v>
-      </c>
-      <c r="AA47" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB47" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC47" s="24"/>
+      <c r="S47" s="38">
+        <v>0</v>
+      </c>
+      <c r="T47" s="38">
+        <v>0</v>
+      </c>
+      <c r="U47" s="38">
+        <v>0</v>
+      </c>
+      <c r="V47" s="38">
+        <v>0</v>
+      </c>
+      <c r="W47" s="47"/>
+      <c r="X47" s="38">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="38">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB47" s="43"/>
+      <c r="AC47" s="45"/>
       <c r="AD47" s="42"/>
-      <c r="AE47" s="2">
-        <v>0</v>
+      <c r="AE47" s="38">
+        <v>1</v>
       </c>
       <c r="AF47" s="45"/>
       <c r="AG47" s="38">
@@ -5567,61 +5616,61 @@
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A48" s="71"/>
-      <c r="B48" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30">
-        <v>0</v>
-      </c>
-      <c r="E48" s="30">
-        <v>0</v>
-      </c>
-      <c r="F48" s="30">
-        <v>0</v>
-      </c>
-      <c r="G48" s="33">
-        <v>0</v>
-      </c>
-      <c r="H48" s="53">
-        <v>1</v>
-      </c>
-      <c r="I48" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="J48" s="30">
-        <v>0</v>
-      </c>
-      <c r="K48" s="55" t="s">
-        <v>155</v>
-      </c>
+      <c r="A48" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="35"/>
+      <c r="D48" s="34">
+        <v>1</v>
+      </c>
+      <c r="E48" s="34">
+        <v>0</v>
+      </c>
+      <c r="F48" s="34">
+        <v>0</v>
+      </c>
+      <c r="G48" s="36">
+        <v>0</v>
+      </c>
+      <c r="H48" s="34">
+        <v>0</v>
+      </c>
+      <c r="I48" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="34">
+        <v>0</v>
+      </c>
+      <c r="K48" s="23"/>
       <c r="L48" s="23"/>
       <c r="M48" s="24"/>
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
       <c r="P48" s="23"/>
-      <c r="Q48" s="30">
+      <c r="Q48" s="34">
         <v>0</v>
       </c>
       <c r="R48" s="24"/>
-      <c r="S48" s="30">
-        <v>0</v>
-      </c>
-      <c r="T48" s="30">
-        <v>0</v>
-      </c>
-      <c r="U48" s="30">
-        <v>0</v>
-      </c>
-      <c r="V48" s="30">
-        <v>1</v>
-      </c>
-      <c r="W48" s="52"/>
-      <c r="X48" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="30">
+      <c r="S48" s="34">
+        <v>0</v>
+      </c>
+      <c r="T48" s="34">
+        <v>0</v>
+      </c>
+      <c r="U48" s="34">
+        <v>0</v>
+      </c>
+      <c r="V48" s="34">
+        <v>0</v>
+      </c>
+      <c r="W48" s="47"/>
+      <c r="X48" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="34">
         <v>0</v>
       </c>
       <c r="Z48" s="62">
@@ -5629,9 +5678,7 @@
       </c>
       <c r="AA48" s="23"/>
       <c r="AB48" s="23"/>
-      <c r="AC48" s="62">
-        <v>1</v>
-      </c>
+      <c r="AC48" s="24"/>
       <c r="AD48" s="42"/>
       <c r="AE48" s="2">
         <v>0</v>
@@ -5642,15 +5689,15 @@
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A49" s="70" t="s">
-        <v>90</v>
+      <c r="A49" s="75" t="s">
+        <v>86</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="20">
         <v>0</v>
@@ -5658,7 +5705,7 @@
       <c r="F49" s="20">
         <v>0</v>
       </c>
-      <c r="G49" s="21">
+      <c r="G49" s="50">
         <v>1</v>
       </c>
       <c r="H49" s="20">
@@ -5670,9 +5717,7 @@
       <c r="J49" s="20">
         <v>0</v>
       </c>
-      <c r="K49" s="55" t="s">
-        <v>156</v>
-      </c>
+      <c r="K49" s="23"/>
       <c r="L49" s="23"/>
       <c r="M49" s="24"/>
       <c r="N49" s="23"/>
@@ -5694,27 +5739,27 @@
       <c r="V49" s="20">
         <v>0</v>
       </c>
-      <c r="W49" s="58" t="s">
-        <v>159</v>
+      <c r="W49" s="49" t="s">
+        <v>143</v>
       </c>
       <c r="X49" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y49" s="20">
         <v>0</v>
       </c>
-      <c r="Z49" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA49" s="23"/>
+      <c r="Z49" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA49" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="AB49" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC49" s="18">
-        <v>0</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="AC49" s="24"/>
       <c r="AD49" s="42"/>
-      <c r="AE49" s="38">
+      <c r="AE49" s="2">
         <v>0</v>
       </c>
       <c r="AF49" s="45"/>
@@ -5723,77 +5768,73 @@
       </c>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A50" s="70"/>
-      <c r="B50" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="2">
-        <v>0</v>
-      </c>
-      <c r="E50" s="2">
-        <v>0</v>
-      </c>
-      <c r="F50" s="2">
-        <v>0</v>
-      </c>
-      <c r="G50" s="3">
-        <v>1</v>
-      </c>
-      <c r="H50" s="2">
-        <v>0</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J50" s="2">
+      <c r="A50" s="75"/>
+      <c r="B50" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="30">
+        <v>0</v>
+      </c>
+      <c r="E50" s="30">
+        <v>0</v>
+      </c>
+      <c r="F50" s="30">
+        <v>0</v>
+      </c>
+      <c r="G50" s="33">
+        <v>0</v>
+      </c>
+      <c r="H50" s="53">
+        <v>1</v>
+      </c>
+      <c r="I50" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="J50" s="30">
         <v>0</v>
       </c>
       <c r="K50" s="55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L50" s="23"/>
       <c r="M50" s="24"/>
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
       <c r="P50" s="23"/>
-      <c r="Q50" s="2">
+      <c r="Q50" s="30">
         <v>0</v>
       </c>
       <c r="R50" s="24"/>
-      <c r="S50" s="2">
-        <v>0</v>
-      </c>
-      <c r="T50" s="2">
-        <v>0</v>
-      </c>
-      <c r="U50" s="2">
-        <v>0</v>
-      </c>
-      <c r="V50" s="2">
-        <v>0</v>
-      </c>
-      <c r="W50" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="X50" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z50" s="2">
+      <c r="S50" s="30">
+        <v>0</v>
+      </c>
+      <c r="T50" s="30">
+        <v>0</v>
+      </c>
+      <c r="U50" s="30">
+        <v>0</v>
+      </c>
+      <c r="V50" s="30">
+        <v>1</v>
+      </c>
+      <c r="W50" s="52"/>
+      <c r="X50" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="62">
         <v>1</v>
       </c>
       <c r="AA50" s="23"/>
-      <c r="AB50" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC50" s="25">
-        <v>0</v>
+      <c r="AB50" s="23"/>
+      <c r="AC50" s="62">
+        <v>1</v>
       </c>
       <c r="AD50" s="42"/>
-      <c r="AE50" s="38">
+      <c r="AE50" s="2">
         <v>0</v>
       </c>
       <c r="AF50" s="45"/>
@@ -5802,76 +5843,76 @@
       </c>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A51" s="70"/>
-      <c r="B51" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="30">
-        <v>0</v>
-      </c>
-      <c r="E51" s="30">
-        <v>0</v>
-      </c>
-      <c r="F51" s="30">
-        <v>0</v>
-      </c>
-      <c r="G51" s="33">
-        <v>1</v>
-      </c>
-      <c r="H51" s="30">
-        <v>0</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="J51" s="30">
-        <v>1</v>
+      <c r="A51" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20">
+        <v>0</v>
+      </c>
+      <c r="E51" s="20">
+        <v>0</v>
+      </c>
+      <c r="F51" s="20">
+        <v>0</v>
+      </c>
+      <c r="G51" s="21">
+        <v>1</v>
+      </c>
+      <c r="H51" s="20">
+        <v>0</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" s="20">
+        <v>0</v>
       </c>
       <c r="K51" s="55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L51" s="23"/>
       <c r="M51" s="24"/>
       <c r="N51" s="23"/>
       <c r="O51" s="23"/>
       <c r="P51" s="23"/>
-      <c r="Q51" s="30">
+      <c r="Q51" s="20">
         <v>0</v>
       </c>
       <c r="R51" s="24"/>
-      <c r="S51" s="30">
-        <v>0</v>
-      </c>
-      <c r="T51" s="30">
-        <v>0</v>
-      </c>
-      <c r="U51" s="30">
-        <v>0</v>
-      </c>
-      <c r="V51" s="30">
-        <v>0</v>
-      </c>
-      <c r="W51" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="X51" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA51" s="38">
-        <v>10</v>
-      </c>
-      <c r="AB51" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC51" s="61" t="s">
-        <v>163</v>
+      <c r="S51" s="20">
+        <v>0</v>
+      </c>
+      <c r="T51" s="20">
+        <v>0</v>
+      </c>
+      <c r="U51" s="20">
+        <v>0</v>
+      </c>
+      <c r="V51" s="20">
+        <v>0</v>
+      </c>
+      <c r="W51" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="X51" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="20">
+        <v>1</v>
+      </c>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC51" s="18">
+        <v>0</v>
       </c>
       <c r="AD51" s="42"/>
       <c r="AE51" s="38">
@@ -5882,189 +5923,193 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="20">
-        <v>0</v>
-      </c>
-      <c r="E52" s="20">
-        <v>0</v>
-      </c>
-      <c r="F52" s="20">
-        <v>0</v>
-      </c>
-      <c r="G52" s="21">
-        <v>1</v>
-      </c>
-      <c r="H52" s="20">
-        <v>0</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J52" s="20">
-        <v>0</v>
-      </c>
-      <c r="K52" s="23"/>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A52" s="74"/>
+      <c r="B52" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="27"/>
+      <c r="D52" s="2">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0</v>
+      </c>
+      <c r="K52" s="55" t="s">
+        <v>156</v>
+      </c>
       <c r="L52" s="23"/>
       <c r="M52" s="24"/>
       <c r="N52" s="23"/>
       <c r="O52" s="23"/>
       <c r="P52" s="23"/>
-      <c r="Q52" s="20">
+      <c r="Q52" s="2">
         <v>0</v>
       </c>
       <c r="R52" s="24"/>
-      <c r="S52" s="20">
-        <v>0</v>
-      </c>
-      <c r="T52" s="20">
-        <v>0</v>
-      </c>
-      <c r="U52" s="20">
-        <v>0</v>
-      </c>
-      <c r="V52" s="20">
-        <v>0</v>
-      </c>
-      <c r="W52" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="X52" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="20">
+      <c r="S52" s="2">
+        <v>0</v>
+      </c>
+      <c r="T52" s="2">
+        <v>0</v>
+      </c>
+      <c r="U52" s="2">
+        <v>0</v>
+      </c>
+      <c r="V52" s="2">
+        <v>0</v>
+      </c>
+      <c r="W52" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="X52" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="2">
         <v>1</v>
       </c>
       <c r="AA52" s="23"/>
-      <c r="AB52" s="69" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC52" s="18">
+      <c r="AB52" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC52" s="25">
         <v>0</v>
       </c>
       <c r="AD52" s="42"/>
       <c r="AE52" s="38">
         <v>0</v>
       </c>
-      <c r="AF52" s="65" t="s">
-        <v>165</v>
-      </c>
+      <c r="AF52" s="45"/>
       <c r="AG52" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A53" s="71"/>
-      <c r="B53" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="2">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2">
-        <v>0</v>
-      </c>
-      <c r="F53" s="2">
-        <v>0</v>
-      </c>
-      <c r="G53" s="3">
-        <v>0</v>
-      </c>
-      <c r="H53" s="2">
-        <v>0</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J53" s="2">
-        <v>0</v>
-      </c>
-      <c r="K53" s="23"/>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A53" s="74"/>
+      <c r="B53" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="29"/>
+      <c r="D53" s="30">
+        <v>0</v>
+      </c>
+      <c r="E53" s="30">
+        <v>0</v>
+      </c>
+      <c r="F53" s="30">
+        <v>0</v>
+      </c>
+      <c r="G53" s="33">
+        <v>1</v>
+      </c>
+      <c r="H53" s="30">
+        <v>0</v>
+      </c>
+      <c r="I53" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" s="30">
+        <v>1</v>
+      </c>
+      <c r="K53" s="55" t="s">
+        <v>157</v>
+      </c>
       <c r="L53" s="23"/>
       <c r="M53" s="24"/>
       <c r="N53" s="23"/>
       <c r="O53" s="23"/>
       <c r="P53" s="23"/>
-      <c r="Q53" s="2">
+      <c r="Q53" s="30">
         <v>0</v>
       </c>
       <c r="R53" s="24"/>
-      <c r="S53" s="2">
-        <v>0</v>
-      </c>
-      <c r="T53" s="2">
-        <v>0</v>
-      </c>
-      <c r="U53" s="2">
-        <v>0</v>
-      </c>
-      <c r="V53" s="2">
-        <v>0</v>
-      </c>
-      <c r="W53" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="X53" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA53" s="23"/>
-      <c r="AB53" s="43"/>
-      <c r="AC53" s="25">
-        <v>0</v>
+      <c r="S53" s="30">
+        <v>0</v>
+      </c>
+      <c r="T53" s="30">
+        <v>0</v>
+      </c>
+      <c r="U53" s="30">
+        <v>0</v>
+      </c>
+      <c r="V53" s="30">
+        <v>0</v>
+      </c>
+      <c r="W53" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="X53" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA53" s="38">
+        <v>10</v>
+      </c>
+      <c r="AB53" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC53" s="61" t="s">
+        <v>163</v>
       </c>
       <c r="AD53" s="42"/>
       <c r="AE53" s="38">
         <v>0</v>
       </c>
-      <c r="AF53" s="65" t="s">
-        <v>166</v>
-      </c>
+      <c r="AF53" s="45"/>
       <c r="AG53" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A54" s="71"/>
-      <c r="B54" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="2">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2">
-        <v>0</v>
-      </c>
-      <c r="F54" s="2">
-        <v>0</v>
-      </c>
-      <c r="G54" s="3">
-        <v>0</v>
-      </c>
-      <c r="H54" s="2">
-        <v>0</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J54" s="2">
+      <c r="A54" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="20">
+        <v>0</v>
+      </c>
+      <c r="E54" s="20">
+        <v>0</v>
+      </c>
+      <c r="F54" s="20">
+        <v>0</v>
+      </c>
+      <c r="G54" s="21">
+        <v>1</v>
+      </c>
+      <c r="H54" s="20">
+        <v>0</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="20">
         <v>0</v>
       </c>
       <c r="K54" s="23"/>
@@ -6073,37 +6118,39 @@
       <c r="N54" s="23"/>
       <c r="O54" s="23"/>
       <c r="P54" s="23"/>
-      <c r="Q54" s="2">
+      <c r="Q54" s="20">
         <v>0</v>
       </c>
       <c r="R54" s="24"/>
-      <c r="S54" s="2">
-        <v>0</v>
-      </c>
-      <c r="T54" s="2">
-        <v>0</v>
-      </c>
-      <c r="U54" s="2">
-        <v>0</v>
-      </c>
-      <c r="V54" s="2">
-        <v>0</v>
-      </c>
-      <c r="W54" s="4" t="s">
+      <c r="S54" s="20">
+        <v>0</v>
+      </c>
+      <c r="T54" s="20">
+        <v>0</v>
+      </c>
+      <c r="U54" s="20">
+        <v>0</v>
+      </c>
+      <c r="V54" s="20">
+        <v>0</v>
+      </c>
+      <c r="W54" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="X54" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="2">
+      <c r="X54" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="20">
         <v>1</v>
       </c>
       <c r="AA54" s="23"/>
-      <c r="AB54" s="43"/>
-      <c r="AC54" s="25">
+      <c r="AB54" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC54" s="18">
         <v>0</v>
       </c>
       <c r="AD54" s="42"/>
@@ -6111,16 +6158,16 @@
         <v>0</v>
       </c>
       <c r="AF54" s="65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AG54" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="71"/>
+      <c r="A55" s="75"/>
       <c r="B55" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C55" s="27"/>
       <c r="D55" s="2">
@@ -6188,16 +6235,16 @@
         <v>0</v>
       </c>
       <c r="AF55" s="65" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AG55" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A56" s="71"/>
+      <c r="A56" s="75"/>
       <c r="B56" s="25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="2">
@@ -6265,16 +6312,16 @@
         <v>0</v>
       </c>
       <c r="AF56" s="65" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AG56" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A57" s="71"/>
+      <c r="A57" s="75"/>
       <c r="B57" s="25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="2">
@@ -6287,7 +6334,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" s="2">
         <v>0</v>
@@ -6333,9 +6380,7 @@
         <v>1</v>
       </c>
       <c r="AA57" s="23"/>
-      <c r="AB57" s="69" t="s">
-        <v>181</v>
-      </c>
+      <c r="AB57" s="43"/>
       <c r="AC57" s="25">
         <v>0</v>
       </c>
@@ -6344,16 +6389,16 @@
         <v>0</v>
       </c>
       <c r="AF57" s="65" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG57" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="71"/>
+      <c r="A58" s="75"/>
       <c r="B58" s="25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C58" s="27"/>
       <c r="D58" s="2">
@@ -6421,16 +6466,16 @@
         <v>0</v>
       </c>
       <c r="AF58" s="65" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AG58" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="71"/>
+      <c r="A59" s="75"/>
       <c r="B59" s="25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="2">
@@ -6500,28 +6545,28 @@
         <v>0</v>
       </c>
       <c r="AF59" s="65" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AG59" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A60" s="71"/>
-      <c r="B60" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30">
-        <v>0</v>
-      </c>
-      <c r="E60" s="30">
-        <v>0</v>
-      </c>
-      <c r="F60" s="30">
-        <v>0</v>
-      </c>
-      <c r="G60" s="33">
+      <c r="A60" s="75"/>
+      <c r="B60" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" s="27"/>
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3">
         <v>0</v>
       </c>
       <c r="H60" s="2">
@@ -6530,7 +6575,7 @@
       <c r="I60" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J60" s="30">
+      <c r="J60" s="2">
         <v>0</v>
       </c>
       <c r="K60" s="23"/>
@@ -6577,114 +6622,108 @@
         <v>0</v>
       </c>
       <c r="AF60" s="65" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AG60" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A61" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="20">
-        <v>0</v>
-      </c>
-      <c r="E61" s="20">
-        <v>0</v>
-      </c>
-      <c r="F61" s="20">
-        <v>1</v>
-      </c>
-      <c r="G61" s="21">
-        <v>1</v>
-      </c>
-      <c r="H61" s="20">
-        <v>0</v>
-      </c>
-      <c r="I61" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J61" s="20">
-        <v>1</v>
-      </c>
-      <c r="K61" s="46" t="s">
-        <v>149</v>
-      </c>
+    <row r="61" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A61" s="75"/>
+      <c r="B61" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="27"/>
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61" s="2">
+        <v>0</v>
+      </c>
+      <c r="K61" s="23"/>
       <c r="L61" s="23"/>
       <c r="M61" s="24"/>
       <c r="N61" s="23"/>
-      <c r="O61" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="P61" s="55"/>
-      <c r="Q61" s="20">
+      <c r="O61" s="23"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="2">
         <v>0</v>
       </c>
       <c r="R61" s="24"/>
-      <c r="S61" s="20">
-        <v>0</v>
-      </c>
-      <c r="T61" s="20">
-        <v>0</v>
-      </c>
-      <c r="U61" s="20">
-        <v>0</v>
-      </c>
-      <c r="V61" s="20">
-        <v>0</v>
-      </c>
-      <c r="W61" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="X61" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="62">
-        <v>1</v>
-      </c>
-      <c r="AA61" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB61" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC61" s="60" t="s">
-        <v>162</v>
+      <c r="S61" s="2">
+        <v>0</v>
+      </c>
+      <c r="T61" s="2">
+        <v>0</v>
+      </c>
+      <c r="U61" s="2">
+        <v>0</v>
+      </c>
+      <c r="V61" s="2">
+        <v>0</v>
+      </c>
+      <c r="W61" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="X61" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="23"/>
+      <c r="AB61" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC61" s="25">
+        <v>0</v>
       </c>
       <c r="AD61" s="42"/>
       <c r="AE61" s="38">
         <v>0</v>
       </c>
-      <c r="AF61" s="45"/>
+      <c r="AF61" s="65" t="s">
+        <v>172</v>
+      </c>
       <c r="AG61" s="38">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A62" s="71"/>
-      <c r="B62" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="2">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2">
-        <v>0</v>
-      </c>
-      <c r="F62" s="2">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3">
-        <v>1</v>
+    <row r="62" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A62" s="75"/>
+      <c r="B62" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="29"/>
+      <c r="D62" s="30">
+        <v>0</v>
+      </c>
+      <c r="E62" s="30">
+        <v>0</v>
+      </c>
+      <c r="F62" s="30">
+        <v>0</v>
+      </c>
+      <c r="G62" s="33">
+        <v>0</v>
       </c>
       <c r="H62" s="2">
         <v>0</v>
@@ -6692,19 +6731,15 @@
       <c r="I62" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J62" s="2">
-        <v>1</v>
-      </c>
-      <c r="K62" s="46" t="s">
-        <v>150</v>
-      </c>
+      <c r="J62" s="30">
+        <v>0</v>
+      </c>
+      <c r="K62" s="23"/>
       <c r="L62" s="23"/>
       <c r="M62" s="24"/>
       <c r="N62" s="23"/>
-      <c r="O62" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="P62" s="55"/>
+      <c r="O62" s="23"/>
+      <c r="P62" s="23"/>
       <c r="Q62" s="2">
         <v>0</v>
       </c>
@@ -6721,8 +6756,8 @@
       <c r="V62" s="2">
         <v>0</v>
       </c>
-      <c r="W62" s="48" t="s">
-        <v>145</v>
+      <c r="W62" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="X62" s="2">
         <v>0</v>
@@ -6730,100 +6765,100 @@
       <c r="Y62" s="2">
         <v>0</v>
       </c>
-      <c r="Z62" s="62">
-        <v>1</v>
-      </c>
-      <c r="AA62" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB62" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC62" s="63" t="s">
-        <v>162</v>
+      <c r="Z62" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA62" s="23"/>
+      <c r="AB62" s="43"/>
+      <c r="AC62" s="25">
+        <v>0</v>
       </c>
       <c r="AD62" s="42"/>
       <c r="AE62" s="38">
         <v>0</v>
       </c>
-      <c r="AF62" s="45"/>
+      <c r="AF62" s="65" t="s">
+        <v>173</v>
+      </c>
       <c r="AG62" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A63" s="71"/>
-      <c r="B63" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="2">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2">
-        <v>0</v>
-      </c>
-      <c r="F63" s="2">
-        <v>1</v>
-      </c>
-      <c r="G63" s="3">
-        <v>1</v>
-      </c>
-      <c r="H63" s="2">
-        <v>0</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J63" s="2">
+      <c r="A63" s="75" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20">
+        <v>0</v>
+      </c>
+      <c r="E63" s="20">
+        <v>0</v>
+      </c>
+      <c r="F63" s="20">
+        <v>1</v>
+      </c>
+      <c r="G63" s="21">
+        <v>1</v>
+      </c>
+      <c r="H63" s="20">
+        <v>0</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J63" s="20">
         <v>1</v>
       </c>
       <c r="K63" s="46" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="L63" s="23"/>
       <c r="M63" s="24"/>
       <c r="N63" s="23"/>
-      <c r="O63" s="57" t="s">
-        <v>83</v>
+      <c r="O63" s="56" t="s">
+        <v>28</v>
       </c>
       <c r="P63" s="55"/>
-      <c r="Q63" s="2">
+      <c r="Q63" s="20">
         <v>0</v>
       </c>
       <c r="R63" s="24"/>
-      <c r="S63" s="2">
-        <v>0</v>
-      </c>
-      <c r="T63" s="2">
-        <v>0</v>
-      </c>
-      <c r="U63" s="2">
-        <v>0</v>
-      </c>
-      <c r="V63" s="2">
-        <v>0</v>
-      </c>
-      <c r="W63" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="X63" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="2">
+      <c r="S63" s="20">
+        <v>0</v>
+      </c>
+      <c r="T63" s="20">
+        <v>0</v>
+      </c>
+      <c r="U63" s="20">
+        <v>0</v>
+      </c>
+      <c r="V63" s="20">
+        <v>0</v>
+      </c>
+      <c r="W63" s="46" t="s">
+        <v>151</v>
+      </c>
+      <c r="X63" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="20">
         <v>0</v>
       </c>
       <c r="Z63" s="62">
         <v>1</v>
       </c>
-      <c r="AA63" s="4" t="s">
+      <c r="AA63" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AB63" s="39" t="s">
+      <c r="AB63" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AC63" s="63" t="s">
-        <v>163</v>
+      <c r="AC63" s="60" t="s">
+        <v>162</v>
       </c>
       <c r="AD63" s="42"/>
       <c r="AE63" s="38">
@@ -6835,9 +6870,9 @@
       </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A64" s="71"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="27"/>
       <c r="D64" s="2">
@@ -6862,13 +6897,13 @@
         <v>1</v>
       </c>
       <c r="K64" s="46" t="s">
-        <v>31</v>
+        <v>150</v>
       </c>
       <c r="L64" s="23"/>
       <c r="M64" s="24"/>
       <c r="N64" s="23"/>
       <c r="O64" s="57" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="P64" s="55"/>
       <c r="Q64" s="2">
@@ -6887,8 +6922,8 @@
       <c r="V64" s="2">
         <v>0</v>
       </c>
-      <c r="W64" s="46" t="s">
-        <v>28</v>
+      <c r="W64" s="48" t="s">
+        <v>145</v>
       </c>
       <c r="X64" s="2">
         <v>0</v>
@@ -6918,9 +6953,9 @@
       </c>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A65" s="71"/>
+      <c r="A65" s="75"/>
       <c r="B65" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C65" s="27"/>
       <c r="D65" s="2">
@@ -6951,7 +6986,7 @@
       <c r="M65" s="24"/>
       <c r="N65" s="23"/>
       <c r="O65" s="57" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="P65" s="55"/>
       <c r="Q65" s="2">
@@ -6971,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="W65" s="48" t="s">
-        <v>28</v>
+        <v>152</v>
       </c>
       <c r="X65" s="2">
         <v>0</v>
@@ -6989,7 +7024,7 @@
         <v>34</v>
       </c>
       <c r="AC65" s="63" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AD65" s="42"/>
       <c r="AE65" s="38">
@@ -7001,22 +7036,22 @@
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A66" s="71"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="2">
         <v>0</v>
       </c>
       <c r="E66" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66" s="2">
         <v>0</v>
@@ -7033,10 +7068,10 @@
       <c r="L66" s="23"/>
       <c r="M66" s="24"/>
       <c r="N66" s="23"/>
-      <c r="O66" s="55"/>
-      <c r="P66" s="57" t="s">
-        <v>28</v>
-      </c>
+      <c r="O66" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="P66" s="55"/>
       <c r="Q66" s="2">
         <v>0</v>
       </c>
@@ -7053,7 +7088,7 @@
       <c r="V66" s="2">
         <v>0</v>
       </c>
-      <c r="W66" s="48" t="s">
+      <c r="W66" s="46" t="s">
         <v>28</v>
       </c>
       <c r="X66" s="2">
@@ -7068,9 +7103,11 @@
       <c r="AA66" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB66" s="43"/>
-      <c r="AC66">
-        <v>0</v>
+      <c r="AB66" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC66" s="63" t="s">
+        <v>162</v>
       </c>
       <c r="AD66" s="42"/>
       <c r="AE66" s="38">
@@ -7082,22 +7119,22 @@
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A67" s="71"/>
+      <c r="A67" s="75"/>
       <c r="B67" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C67" s="27"/>
       <c r="D67" s="2">
         <v>0</v>
       </c>
       <c r="E67" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="2">
         <v>0</v>
@@ -7114,10 +7151,10 @@
       <c r="L67" s="23"/>
       <c r="M67" s="24"/>
       <c r="N67" s="23"/>
-      <c r="O67" s="55"/>
-      <c r="P67" s="57" t="s">
-        <v>60</v>
-      </c>
+      <c r="O67" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="P67" s="55"/>
       <c r="Q67" s="2">
         <v>0</v>
       </c>
@@ -7134,7 +7171,7 @@
       <c r="V67" s="2">
         <v>0</v>
       </c>
-      <c r="W67" s="46" t="s">
+      <c r="W67" s="48" t="s">
         <v>28</v>
       </c>
       <c r="X67" s="2">
@@ -7149,9 +7186,11 @@
       <c r="AA67" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB67" s="43"/>
-      <c r="AC67">
-        <v>0</v>
+      <c r="AB67" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC67" s="63" t="s">
+        <v>162</v>
       </c>
       <c r="AD67" s="42"/>
       <c r="AE67" s="38">
@@ -7163,9 +7202,9 @@
       </c>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A68" s="71"/>
+      <c r="A68" s="75"/>
       <c r="B68" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C68" s="27"/>
       <c r="D68" s="2">
@@ -7197,7 +7236,7 @@
       <c r="N68" s="23"/>
       <c r="O68" s="55"/>
       <c r="P68" s="57" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="Q68" s="2">
         <v>0</v>
@@ -7244,22 +7283,22 @@
       </c>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A69" s="71"/>
+      <c r="A69" s="75"/>
       <c r="B69" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="2">
         <v>0</v>
       </c>
       <c r="E69" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G69" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" s="2">
         <v>0</v>
@@ -7276,10 +7315,10 @@
       <c r="L69" s="23"/>
       <c r="M69" s="24"/>
       <c r="N69" s="23"/>
-      <c r="O69" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="P69" s="55"/>
+      <c r="O69" s="55"/>
+      <c r="P69" s="57" t="s">
+        <v>60</v>
+      </c>
       <c r="Q69" s="2">
         <v>0</v>
       </c>
@@ -7296,7 +7335,7 @@
       <c r="V69" s="2">
         <v>0</v>
       </c>
-      <c r="W69" s="48" t="s">
+      <c r="W69" s="46" t="s">
         <v>28</v>
       </c>
       <c r="X69" s="2">
@@ -7311,11 +7350,9 @@
       <c r="AA69" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB69" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC69" s="63" t="s">
-        <v>162</v>
+      <c r="AB69" s="43"/>
+      <c r="AC69">
+        <v>0</v>
       </c>
       <c r="AD69" s="42"/>
       <c r="AE69" s="38">
@@ -7327,22 +7364,22 @@
       </c>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A70" s="71"/>
+      <c r="A70" s="75"/>
       <c r="B70" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C70" s="27"/>
       <c r="D70" s="2">
         <v>0</v>
       </c>
       <c r="E70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G70" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" s="2">
         <v>0</v>
@@ -7359,10 +7396,10 @@
       <c r="L70" s="23"/>
       <c r="M70" s="24"/>
       <c r="N70" s="23"/>
-      <c r="O70" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="P70" s="55"/>
+      <c r="O70" s="55"/>
+      <c r="P70" s="57" t="s">
+        <v>83</v>
+      </c>
       <c r="Q70" s="2">
         <v>0</v>
       </c>
@@ -7379,7 +7416,7 @@
       <c r="V70" s="2">
         <v>0</v>
       </c>
-      <c r="W70" s="46" t="s">
+      <c r="W70" s="48" t="s">
         <v>28</v>
       </c>
       <c r="X70" s="2">
@@ -7394,11 +7431,9 @@
       <c r="AA70" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB70" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC70" s="63" t="s">
-        <v>162</v>
+      <c r="AB70" s="43"/>
+      <c r="AC70">
+        <v>0</v>
       </c>
       <c r="AD70" s="42"/>
       <c r="AE70" s="38">
@@ -7410,22 +7445,22 @@
       </c>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A71" s="71"/>
+      <c r="A71" s="75"/>
       <c r="B71" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C71" s="27"/>
       <c r="D71" s="2">
         <v>0</v>
       </c>
       <c r="E71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71" s="2">
         <v>0</v>
@@ -7442,10 +7477,10 @@
       <c r="L71" s="23"/>
       <c r="M71" s="24"/>
       <c r="N71" s="23"/>
-      <c r="O71" s="55"/>
-      <c r="P71" s="57" t="s">
-        <v>75</v>
-      </c>
+      <c r="O71" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="P71" s="55"/>
       <c r="Q71" s="2">
         <v>0</v>
       </c>
@@ -7477,9 +7512,11 @@
       <c r="AA71" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB71" s="43"/>
-      <c r="AC71">
-        <v>0</v>
+      <c r="AB71" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC71" s="63" t="s">
+        <v>162</v>
       </c>
       <c r="AD71" s="42"/>
       <c r="AE71" s="38">
@@ -7491,22 +7528,22 @@
       </c>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A72" s="71"/>
-      <c r="B72" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30">
-        <v>0</v>
-      </c>
-      <c r="E72" s="30">
-        <v>1</v>
-      </c>
-      <c r="F72" s="30">
-        <v>0</v>
-      </c>
-      <c r="G72" s="33">
-        <v>0</v>
+      <c r="A72" s="75"/>
+      <c r="B72" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" s="27"/>
+      <c r="D72" s="2">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>1</v>
+      </c>
+      <c r="G72" s="3">
+        <v>1</v>
       </c>
       <c r="H72" s="2">
         <v>0</v>
@@ -7523,10 +7560,10 @@
       <c r="L72" s="23"/>
       <c r="M72" s="24"/>
       <c r="N72" s="23"/>
-      <c r="O72" s="55"/>
-      <c r="P72" s="54" t="s">
-        <v>77</v>
-      </c>
+      <c r="O72" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="P72" s="55"/>
       <c r="Q72" s="2">
         <v>0</v>
       </c>
@@ -7543,7 +7580,7 @@
       <c r="V72" s="2">
         <v>0</v>
       </c>
-      <c r="W72" s="48" t="s">
+      <c r="W72" s="46" t="s">
         <v>28</v>
       </c>
       <c r="X72" s="2">
@@ -7558,9 +7595,11 @@
       <c r="AA72" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AB72" s="43"/>
-      <c r="AC72">
-        <v>0</v>
+      <c r="AB72" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC72" s="63" t="s">
+        <v>162</v>
       </c>
       <c r="AD72" s="42"/>
       <c r="AE72" s="38">
@@ -7572,73 +7611,75 @@
       </c>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A73" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C73" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="D73" s="20">
-        <v>0</v>
-      </c>
-      <c r="E73" s="20">
-        <v>0</v>
-      </c>
-      <c r="F73" s="20">
-        <v>0</v>
-      </c>
-      <c r="G73" s="21">
-        <v>1</v>
-      </c>
-      <c r="H73" s="20">
-        <v>0</v>
-      </c>
-      <c r="I73" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="J73" s="20">
-        <v>0</v>
-      </c>
-      <c r="K73" s="23"/>
+      <c r="A73" s="75"/>
+      <c r="B73" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="27"/>
+      <c r="D73" s="2">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0</v>
+      </c>
+      <c r="H73" s="2">
+        <v>0</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J73" s="2">
+        <v>1</v>
+      </c>
+      <c r="K73" s="46" t="s">
+        <v>31</v>
+      </c>
       <c r="L73" s="23"/>
       <c r="M73" s="24"/>
       <c r="N73" s="23"/>
-      <c r="O73" s="23"/>
-      <c r="P73" s="23"/>
-      <c r="Q73" s="20">
+      <c r="O73" s="55"/>
+      <c r="P73" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q73" s="2">
         <v>0</v>
       </c>
       <c r="R73" s="24"/>
-      <c r="S73" s="20">
-        <v>0</v>
-      </c>
-      <c r="T73" s="20">
-        <v>0</v>
-      </c>
-      <c r="U73" s="20">
-        <v>0</v>
-      </c>
-      <c r="V73" s="20">
-        <v>0</v>
-      </c>
-      <c r="W73" s="45"/>
-      <c r="X73" s="20">
-        <v>0</v>
-      </c>
-      <c r="Y73" s="20">
-        <v>0</v>
-      </c>
-      <c r="Z73" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA73" s="23"/>
-      <c r="AB73" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC73" s="18">
+      <c r="S73" s="2">
+        <v>0</v>
+      </c>
+      <c r="T73" s="2">
+        <v>0</v>
+      </c>
+      <c r="U73" s="2">
+        <v>0</v>
+      </c>
+      <c r="V73" s="2">
+        <v>0</v>
+      </c>
+      <c r="W73" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="X73" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA73" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB73" s="43"/>
+      <c r="AC73">
         <v>0</v>
       </c>
       <c r="AD73" s="42"/>
@@ -7651,21 +7692,21 @@
       </c>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A74" s="71"/>
-      <c r="B74" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C74" s="27"/>
-      <c r="D74" s="2">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2">
-        <v>0</v>
-      </c>
-      <c r="F74" s="2">
-        <v>0</v>
-      </c>
-      <c r="G74" s="3">
+      <c r="A74" s="75"/>
+      <c r="B74" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C74" s="29"/>
+      <c r="D74" s="30">
+        <v>0</v>
+      </c>
+      <c r="E74" s="30">
+        <v>1</v>
+      </c>
+      <c r="F74" s="30">
+        <v>0</v>
+      </c>
+      <c r="G74" s="33">
         <v>0</v>
       </c>
       <c r="H74" s="2">
@@ -7675,22 +7716,24 @@
         <v>28</v>
       </c>
       <c r="J74" s="2">
-        <v>0</v>
-      </c>
-      <c r="K74" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="K74" s="46" t="s">
+        <v>31</v>
+      </c>
       <c r="L74" s="23"/>
       <c r="M74" s="24"/>
       <c r="N74" s="23"/>
-      <c r="O74" s="23"/>
-      <c r="P74" s="23"/>
+      <c r="O74" s="55"/>
+      <c r="P74" s="54" t="s">
+        <v>77</v>
+      </c>
       <c r="Q74" s="2">
         <v>0</v>
       </c>
-      <c r="R74" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="R74" s="24"/>
       <c r="S74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T74" s="2">
         <v>0</v>
@@ -7701,19 +7744,23 @@
       <c r="V74" s="2">
         <v>0</v>
       </c>
-      <c r="W74" s="45"/>
+      <c r="W74" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="X74" s="2">
         <v>0</v>
       </c>
       <c r="Y74" s="2">
         <v>0</v>
       </c>
-      <c r="Z74" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA74" s="23"/>
+      <c r="Z74" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA74" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AB74" s="43"/>
-      <c r="AC74" s="25">
+      <c r="AC74">
         <v>0</v>
       </c>
       <c r="AD74" s="42"/>
@@ -7726,30 +7773,34 @@
       </c>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A75" s="71"/>
-      <c r="B75" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="27"/>
-      <c r="D75" s="2">
-        <v>0</v>
-      </c>
-      <c r="E75" s="2">
-        <v>0</v>
-      </c>
-      <c r="F75" s="2">
-        <v>0</v>
-      </c>
-      <c r="G75" s="3">
-        <v>0</v>
-      </c>
-      <c r="H75" s="2">
-        <v>0</v>
-      </c>
-      <c r="I75" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J75" s="2">
+      <c r="A75" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="20">
+        <v>0</v>
+      </c>
+      <c r="E75" s="20">
+        <v>0</v>
+      </c>
+      <c r="F75" s="20">
+        <v>0</v>
+      </c>
+      <c r="G75" s="21">
+        <v>1</v>
+      </c>
+      <c r="H75" s="20">
+        <v>0</v>
+      </c>
+      <c r="I75" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J75" s="20">
         <v>0</v>
       </c>
       <c r="K75" s="23"/>
@@ -7758,35 +7809,39 @@
       <c r="N75" s="23"/>
       <c r="O75" s="23"/>
       <c r="P75" s="23"/>
-      <c r="Q75" s="2">
+      <c r="Q75" s="20">
         <v>0</v>
       </c>
       <c r="R75" s="24"/>
-      <c r="S75" s="2">
-        <v>0</v>
-      </c>
-      <c r="T75" s="2">
-        <v>1</v>
-      </c>
-      <c r="U75" s="2">
-        <v>0</v>
-      </c>
-      <c r="V75" s="2">
+      <c r="S75" s="20">
+        <v>0</v>
+      </c>
+      <c r="T75" s="20">
+        <v>0</v>
+      </c>
+      <c r="U75" s="20">
+        <v>0</v>
+      </c>
+      <c r="V75" s="20">
         <v>0</v>
       </c>
       <c r="W75" s="45"/>
-      <c r="X75" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y75" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z75" s="62">
-        <v>1</v>
+      <c r="X75" s="20">
+        <v>0</v>
+      </c>
+      <c r="Y75" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z75" s="20">
+        <v>0</v>
       </c>
       <c r="AA75" s="23"/>
-      <c r="AB75" s="43"/>
-      <c r="AC75" s="24"/>
+      <c r="AB75" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC75" s="18">
+        <v>0</v>
+      </c>
       <c r="AD75" s="42"/>
       <c r="AE75" s="38">
         <v>0</v>
@@ -7797,30 +7852,30 @@
       </c>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A76" s="71"/>
-      <c r="B76" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="30">
-        <v>0</v>
-      </c>
-      <c r="E76" s="30">
-        <v>0</v>
-      </c>
-      <c r="F76" s="30">
-        <v>0</v>
-      </c>
-      <c r="G76" s="33">
-        <v>0</v>
-      </c>
-      <c r="H76" s="30">
-        <v>0</v>
-      </c>
-      <c r="I76" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="J76" s="30">
+      <c r="A76" s="75"/>
+      <c r="B76" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="2">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0</v>
+      </c>
+      <c r="G76" s="3">
+        <v>0</v>
+      </c>
+      <c r="H76" s="2">
+        <v>0</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J76" s="2">
         <v>0</v>
       </c>
       <c r="K76" s="23"/>
@@ -7829,35 +7884,39 @@
       <c r="N76" s="23"/>
       <c r="O76" s="23"/>
       <c r="P76" s="23"/>
-      <c r="Q76" s="30">
-        <v>0</v>
-      </c>
-      <c r="R76" s="24"/>
-      <c r="S76" s="30">
-        <v>0</v>
-      </c>
-      <c r="T76" s="30">
-        <v>0</v>
-      </c>
-      <c r="U76" s="30">
-        <v>1</v>
-      </c>
-      <c r="V76" s="30">
+      <c r="Q76" s="2">
+        <v>0</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="S76" s="2">
+        <v>1</v>
+      </c>
+      <c r="T76" s="2">
+        <v>0</v>
+      </c>
+      <c r="U76" s="2">
+        <v>0</v>
+      </c>
+      <c r="V76" s="2">
         <v>0</v>
       </c>
       <c r="W76" s="45"/>
-      <c r="X76" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y76" s="30">
-        <v>0</v>
-      </c>
-      <c r="Z76" s="62">
+      <c r="X76" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="2">
         <v>1</v>
       </c>
       <c r="AA76" s="23"/>
       <c r="AB76" s="43"/>
-      <c r="AC76" s="24"/>
+      <c r="AC76" s="25">
+        <v>0</v>
+      </c>
       <c r="AD76" s="42"/>
       <c r="AE76" s="38">
         <v>0</v>
@@ -7867,128 +7926,270 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A77" s="68" t="s">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A77" s="75"/>
+      <c r="B77" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" s="27"/>
+      <c r="D77" s="2">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3">
+        <v>0</v>
+      </c>
+      <c r="H77" s="2">
+        <v>0</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J77" s="2">
+        <v>0</v>
+      </c>
+      <c r="K77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="24"/>
+      <c r="N77" s="23"/>
+      <c r="O77" s="23"/>
+      <c r="P77" s="23"/>
+      <c r="Q77" s="2">
+        <v>0</v>
+      </c>
+      <c r="R77" s="24"/>
+      <c r="S77" s="2">
+        <v>0</v>
+      </c>
+      <c r="T77" s="2">
+        <v>1</v>
+      </c>
+      <c r="U77" s="2">
+        <v>0</v>
+      </c>
+      <c r="V77" s="2">
+        <v>0</v>
+      </c>
+      <c r="W77" s="45"/>
+      <c r="X77" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z77" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA77" s="23"/>
+      <c r="AB77" s="43"/>
+      <c r="AC77" s="24"/>
+      <c r="AD77" s="42"/>
+      <c r="AE77" s="38">
+        <v>0</v>
+      </c>
+      <c r="AF77" s="45"/>
+      <c r="AG77" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A78" s="75"/>
+      <c r="B78" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="32"/>
+      <c r="D78" s="30">
+        <v>0</v>
+      </c>
+      <c r="E78" s="30">
+        <v>0</v>
+      </c>
+      <c r="F78" s="30">
+        <v>0</v>
+      </c>
+      <c r="G78" s="33">
+        <v>0</v>
+      </c>
+      <c r="H78" s="30">
+        <v>0</v>
+      </c>
+      <c r="I78" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J78" s="30">
+        <v>0</v>
+      </c>
+      <c r="K78" s="23"/>
+      <c r="L78" s="23"/>
+      <c r="M78" s="24"/>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23"/>
+      <c r="P78" s="23"/>
+      <c r="Q78" s="30">
+        <v>0</v>
+      </c>
+      <c r="R78" s="24"/>
+      <c r="S78" s="30">
+        <v>0</v>
+      </c>
+      <c r="T78" s="30">
+        <v>0</v>
+      </c>
+      <c r="U78" s="30">
+        <v>1</v>
+      </c>
+      <c r="V78" s="30">
+        <v>0</v>
+      </c>
+      <c r="W78" s="45"/>
+      <c r="X78" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="62">
+        <v>1</v>
+      </c>
+      <c r="AA78" s="23"/>
+      <c r="AB78" s="43"/>
+      <c r="AC78" s="24"/>
+      <c r="AD78" s="42"/>
+      <c r="AE78" s="38">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="45"/>
+      <c r="AG78" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:33" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A79" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="B77" s="34" t="s">
+      <c r="B79" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="C77" s="40">
-        <v>0</v>
-      </c>
-      <c r="D77" s="34">
-        <v>0</v>
-      </c>
-      <c r="E77" s="34">
-        <v>0</v>
-      </c>
-      <c r="F77" s="34">
-        <v>0</v>
-      </c>
-      <c r="G77" s="36">
-        <v>0</v>
-      </c>
-      <c r="H77" s="34">
-        <v>0</v>
-      </c>
-      <c r="I77" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="J77" s="34">
-        <v>0</v>
-      </c>
-      <c r="K77" s="37" t="s">
+      <c r="C79" s="40">
+        <v>0</v>
+      </c>
+      <c r="D79" s="34">
+        <v>0</v>
+      </c>
+      <c r="E79" s="34">
+        <v>0</v>
+      </c>
+      <c r="F79" s="34">
+        <v>0</v>
+      </c>
+      <c r="G79" s="36">
+        <v>0</v>
+      </c>
+      <c r="H79" s="34">
+        <v>0</v>
+      </c>
+      <c r="I79" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="J79" s="34">
+        <v>0</v>
+      </c>
+      <c r="K79" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L77" s="37" t="s">
+      <c r="L79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="M77" s="34">
-        <v>0</v>
-      </c>
-      <c r="N77" s="37" t="s">
+      <c r="M79" s="34">
+        <v>0</v>
+      </c>
+      <c r="N79" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="O77" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="P77" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q77" s="34">
-        <v>0</v>
-      </c>
-      <c r="R77" s="37" t="s">
+      <c r="O79" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="P79" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q79" s="34">
+        <v>0</v>
+      </c>
+      <c r="R79" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="S77" s="34">
-        <v>0</v>
-      </c>
-      <c r="T77" s="34">
-        <v>0</v>
-      </c>
-      <c r="U77" s="34">
-        <v>0</v>
-      </c>
-      <c r="V77" s="34">
-        <v>0</v>
-      </c>
-      <c r="W77" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="X77" s="34">
-        <v>0</v>
-      </c>
-      <c r="Y77" s="34">
-        <v>0</v>
-      </c>
-      <c r="Z77" s="34">
-        <v>1</v>
-      </c>
-      <c r="AA77" s="37" t="s">
+      <c r="S79" s="34">
+        <v>0</v>
+      </c>
+      <c r="T79" s="34">
+        <v>0</v>
+      </c>
+      <c r="U79" s="34">
+        <v>0</v>
+      </c>
+      <c r="V79" s="34">
+        <v>0</v>
+      </c>
+      <c r="W79" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="X79" s="34">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="34">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA79" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AB77" s="37" t="s">
+      <c r="AB79" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="AC77" s="41">
-        <v>0</v>
-      </c>
-      <c r="AD77" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE77" s="38">
-        <v>0</v>
-      </c>
-      <c r="AF77" s="45"/>
-      <c r="AG77" s="2">
+      <c r="AC79" s="41">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="38">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="45"/>
+      <c r="AG79" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A80" s="75" t="s">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A82" s="70" t="s">
         <v>188</v>
       </c>
-      <c r="B80" s="76" t="s">
+      <c r="B82" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="Z80" s="76" t="s">
+      <c r="Z82" s="71" t="s">
         <v>189</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A60"/>
-    <mergeCell ref="A61:A72"/>
-    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A54:A62"/>
+    <mergeCell ref="A63:A74"/>
+    <mergeCell ref="A75:A78"/>
     <mergeCell ref="A2:A18"/>
     <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A36:A47"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>